<commit_message>
Almost doen with the Grad stuff
Mostly just the styling is left and maybe some refactoring after we finally demo this bad bay
</commit_message>
<xml_diff>
--- a/GradApp.xlsx
+++ b/GradApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>As a Graduate</t>
   </si>
@@ -113,10 +113,18 @@
     <t>Add start and end date to rotations table for rotation period</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Styling</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>Almost</t>
+  </si>
+  <si>
+    <t>Redirect to GraduatProjectWishLists page for graduate wishlist view
+Indicate if request on project has previously been sent
+Styling</t>
   </si>
 </sst>
 </file>
@@ -197,12 +205,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
@@ -520,37 +531,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="1" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="1" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -558,22 +577,26 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -581,22 +604,26 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -604,22 +631,26 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -627,22 +658,26 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -650,22 +685,26 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -673,82 +712,98 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4">
         <v>9</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -758,22 +813,24 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="4">
+      <c r="D11" s="2"/>
+      <c r="F11" s="4">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -803,8 +860,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C2:D11">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Finalised most of the UI
</commit_message>
<xml_diff>
--- a/GradApp.xlsx
+++ b/GradApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>As a Graduate</t>
   </si>
@@ -125,13 +125,19 @@
     <t>Redirect to GraduatProjectWishLists page for graduate wishlist view
 Indicate if request on project has previously been sent
 Styling</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Text needs to change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +166,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +202,11 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,25 +217,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -534,7 +569,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,314 +585,396 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4">
-        <v>9</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="4"/>
+      <c r="H10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="F11" s="4">
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8">
         <v>10</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="4"/>
+      <c r="H11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D11">

</xml_diff>

<commit_message>
Updated the graduate view
</commit_message>
<xml_diff>
--- a/GradApp.xlsx
+++ b/GradApp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>As a Graduate</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Text needs to change</t>
+  </si>
+  <si>
+    <t>Add skills to the graduate table</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -826,10 +829,10 @@
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="3"/>
       <c r="F11" s="7">
         <v>10</v>
@@ -956,6 +959,14 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D11">

</xml_diff>